<commit_message>
forest goblin wb update
</commit_message>
<xml_diff>
--- a/Players/Kai/nonplayed/forest goblins/forest_goblins_underdog.xlsx
+++ b/Players/Kai/nonplayed/forest goblins/forest_goblins_underdog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klaute\Dropbox\Privat\Mordheim\Players\Kai\nonplayed\forest goblins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD0C3CA-D60C-4EBA-9BA2-19F73FCDC42A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B26CD0F-D936-4530-BC60-56E3DC034FEE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -771,18 +771,6 @@
   </cellStyleXfs>
   <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -832,6 +820,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1196,8 +1196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1223,113 +1223,113 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="7">
-        <v>43606</v>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="3">
+        <v>43640</v>
       </c>
       <c r="I2" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="4">
         <f>J3+(3*'Hired swords'!B5)+H38+I38+J38</f>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="10"/>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6"/>
       <c r="I3" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="7">
         <f>E18+'Hired swords'!B19</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.2">
       <c r="I4" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="8">
         <f>'Characteristic analysis'!J29+'Hired swords'!O19</f>
-        <v>258</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="10">
         <v>500</v>
       </c>
       <c r="I5" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="4">
         <f>E13*10</f>
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="9">
         <f>G18+N42+'Hired swords'!G19</f>
-        <v>312</v>
-      </c>
-      <c r="I6" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="9">
         <f>5*(E18-E17)+E11*F11+E12*F12+E13*F13+E14*F14+E15*F15+E16*F16+E17*20+SUM(H38:J38)*10+'Hired swords'!I19</f>
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="11">
         <f>C5-C6</f>
-        <v>188</v>
+        <v>203</v>
       </c>
       <c r="I7" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="9">
         <f>ROUNDUP(J3/4,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C8">
         <f>'Hired swords'!H19</f>
-        <v>15</v>
-      </c>
-      <c r="I8" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8" s="13">
         <f>Q42</f>
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="K8">
         <f>Q43</f>
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="L8">
         <f>Q44</f>
@@ -1337,30 +1337,30 @@
       </c>
     </row>
     <row r="9" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="J9" s="11">
+      <c r="J9" s="7">
         <f>(J4+J5+J6+J8)*J7</f>
-        <v>360</v>
+        <v>334</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="36" t="s">
         <v>19</v>
       </c>
       <c r="C11" t="s">
@@ -1369,10 +1369,10 @@
       <c r="D11">
         <v>50</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="15">
         <v>1</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="15">
         <v>17</v>
       </c>
       <c r="G11">
@@ -1381,28 +1381,28 @@
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B12" s="4"/>
-      <c r="C12" s="5" t="s">
+      <c r="B12" s="36"/>
+      <c r="C12" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D12">
         <v>20</v>
       </c>
-      <c r="E12" s="19">
-        <v>0</v>
-      </c>
-      <c r="F12" s="19">
+      <c r="E12" s="15">
+        <v>0</v>
+      </c>
+      <c r="F12" s="15">
         <v>6</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="8" t="s">
+      <c r="J12" s="37"/>
+      <c r="K12" s="4" t="s">
         <v>23</v>
       </c>
       <c r="N12" t="s">
@@ -1413,17 +1413,17 @@
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B13" s="4"/>
+      <c r="B13" s="36"/>
       <c r="C13" t="s">
         <v>26</v>
       </c>
       <c r="D13">
         <v>20</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="15">
         <v>1</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="15">
         <v>6</v>
       </c>
       <c r="G13">
@@ -1432,9 +1432,9 @@
       </c>
       <c r="I13">
         <f>J6+J6*50%</f>
-        <v>102</v>
-      </c>
-      <c r="J13" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K13">
@@ -1448,7 +1448,7 @@
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="36" t="s">
         <v>30</v>
       </c>
       <c r="C14" t="s">
@@ -1457,21 +1457,21 @@
       <c r="D14">
         <v>15</v>
       </c>
-      <c r="E14" s="19">
-        <v>0</v>
-      </c>
-      <c r="F14" s="19">
+      <c r="E14" s="15">
+        <v>0</v>
+      </c>
+      <c r="F14" s="15">
         <v>0</v>
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="1">
         <f>J6+J6*75%</f>
-        <v>119</v>
-      </c>
-      <c r="J14" s="5" t="s">
+        <v>101.5</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>32</v>
       </c>
       <c r="N14" t="s">
@@ -1482,28 +1482,28 @@
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B15" s="4"/>
+      <c r="B15" s="36"/>
       <c r="C15" t="s">
         <v>34</v>
       </c>
       <c r="D15">
         <v>20</v>
       </c>
-      <c r="E15" s="19">
+      <c r="E15" s="15">
         <v>1</v>
       </c>
-      <c r="F15" s="19">
+      <c r="F15" s="15">
         <v>0</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I15" s="1">
         <f>J6+J6*100%</f>
-        <v>136</v>
-      </c>
-      <c r="J15" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>35</v>
       </c>
       <c r="N15" t="s">
@@ -1514,149 +1514,149 @@
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B16" s="4"/>
+      <c r="B16" s="36"/>
       <c r="C16" t="s">
         <v>38</v>
       </c>
       <c r="D16">
         <v>25</v>
       </c>
-      <c r="E16" s="19">
-        <v>0</v>
-      </c>
-      <c r="F16" s="19">
+      <c r="E16" s="15">
+        <v>0</v>
+      </c>
+      <c r="F16" s="15">
         <v>0</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I16" s="1">
         <f>J6+J6*150%</f>
-        <v>170</v>
-      </c>
-      <c r="J16" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B17" s="4"/>
-      <c r="C17" s="16" t="s">
+      <c r="B17" s="36"/>
+      <c r="C17" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D17" s="16">
         <v>200</v>
       </c>
-      <c r="E17" s="21">
-        <v>0</v>
-      </c>
-      <c r="F17" s="21">
-        <v>0</v>
-      </c>
-      <c r="G17" s="20">
+      <c r="E17" s="17">
+        <v>0</v>
+      </c>
+      <c r="F17" s="17">
+        <v>0</v>
+      </c>
+      <c r="G17" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I17">
         <f>J6+J6*300%</f>
-        <v>272</v>
-      </c>
-      <c r="J17" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="J17" s="18" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="18" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="7">
         <f>SUM(E11:E17)+C44</f>
         <v>3</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="7">
         <f>SUM(G11:G17)</f>
         <v>90</v>
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B19" s="24"/>
-      <c r="F19" s="8"/>
-      <c r="I19" s="2" t="s">
+      <c r="B19" s="20"/>
+      <c r="F19" s="4"/>
+      <c r="I19" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="38"/>
     </row>
     <row r="20" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="I20" s="2" t="s">
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="I20" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2" t="s">
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="38"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D21" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="25" t="s">
+      <c r="E21" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F21" s="25" t="s">
+      <c r="F21" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="G21" s="18" t="s">
+      <c r="G21" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="H21" s="18" t="str">
+      <c r="H21" s="14" t="str">
         <f>C11</f>
         <v>Chief</v>
       </c>
-      <c r="I21" s="18" t="str">
+      <c r="I21" s="14" t="str">
         <f>C12</f>
         <v>Braves (¾)</v>
       </c>
-      <c r="J21" s="18" t="str">
+      <c r="J21" s="14" t="str">
         <f>C13</f>
         <v>Shaman</v>
       </c>
-      <c r="K21" s="18" t="str">
+      <c r="K21" s="14" t="str">
         <f>C14</f>
         <v>forest goblins</v>
       </c>
-      <c r="L21" s="18" t="str">
+      <c r="L21" s="14" t="str">
         <f>C15</f>
         <v>Shootaz (5)</v>
       </c>
-      <c r="M21" s="18" t="str">
+      <c r="M21" s="14" t="str">
         <f>C16</f>
         <v>red toof goblinz (5)</v>
       </c>
-      <c r="N21" s="18" t="s">
+      <c r="N21" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="O21" s="18" t="s">
+      <c r="O21" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="P21" s="18" t="s">
+      <c r="P21" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="Q21" s="18" t="s">
+      <c r="Q21" s="14" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1667,10 +1667,10 @@
       <c r="C22" t="s">
         <v>56</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="E22" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="1" t="s">
         <v>58</v>
       </c>
       <c r="G22">
@@ -1704,13 +1704,13 @@
         <f t="shared" ref="N22:N40" si="1">SUM(H22:M22)*G22</f>
         <v>0</v>
       </c>
-      <c r="O22" s="5" t="s">
+      <c r="O22" s="1" t="s">
         <v>59</v>
       </c>
       <c r="P22">
         <v>1</v>
       </c>
-      <c r="Q22" s="5">
+      <c r="Q22" s="1">
         <f t="shared" ref="Q22:Q40" si="2">P22*SUM(H22:M22)</f>
         <v>3</v>
       </c>
@@ -1722,10 +1722,10 @@
       <c r="C23" t="s">
         <v>56</v>
       </c>
-      <c r="E23" s="26" t="s">
+      <c r="E23" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="1" t="s">
         <v>58</v>
       </c>
       <c r="G23">
@@ -1755,13 +1755,13 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="O23" s="5" t="s">
+      <c r="O23" s="1" t="s">
         <v>59</v>
       </c>
       <c r="P23">
         <v>1</v>
       </c>
-      <c r="Q23" s="5">
+      <c r="Q23" s="1">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -1773,10 +1773,10 @@
       <c r="C24" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="26" t="s">
+      <c r="E24" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="1" t="s">
         <v>62</v>
       </c>
       <c r="G24">
@@ -1804,13 +1804,13 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O24" s="5" t="s">
+      <c r="O24" s="1" t="s">
         <v>59</v>
       </c>
       <c r="P24">
         <v>3</v>
       </c>
-      <c r="Q24" s="5">
+      <c r="Q24" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1819,13 +1819,13 @@
       <c r="B25" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E25" s="26" t="s">
+      <c r="E25" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="1" t="s">
         <v>64</v>
       </c>
       <c r="G25">
@@ -1853,13 +1853,13 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O25" s="5" t="s">
+      <c r="O25" s="1" t="s">
         <v>65</v>
       </c>
       <c r="P25">
         <v>4</v>
       </c>
-      <c r="Q25" s="5">
+      <c r="Q25" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1868,20 +1868,20 @@
       <c r="B26" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E26" s="26" t="s">
+      <c r="E26" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="1" t="s">
         <v>67</v>
       </c>
       <c r="G26">
         <v>5</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -1900,30 +1900,30 @@
       </c>
       <c r="N26">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O26" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="O26" s="1" t="s">
         <v>59</v>
       </c>
       <c r="P26">
         <v>4</v>
       </c>
-      <c r="Q26" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
+      <c r="Q26" s="1">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E27" s="26" t="s">
+      <c r="E27" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="1" t="s">
         <v>69</v>
       </c>
       <c r="G27">
@@ -1951,13 +1951,13 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O27" s="5" t="s">
+      <c r="O27" s="1" t="s">
         <v>59</v>
       </c>
       <c r="P27">
         <v>4</v>
       </c>
-      <c r="Q27" s="5">
+      <c r="Q27" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1966,13 +1966,13 @@
       <c r="B28" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E28" s="26" t="s">
+      <c r="E28" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="1" t="s">
         <v>72</v>
       </c>
       <c r="G28">
@@ -2001,13 +2001,13 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O28" s="5" t="s">
+      <c r="O28" s="1" t="s">
         <v>65</v>
       </c>
       <c r="P28">
         <v>4</v>
       </c>
-      <c r="Q28" s="5">
+      <c r="Q28" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2016,13 +2016,13 @@
       <c r="B29" t="s">
         <v>73</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E29" s="26" t="s">
+      <c r="E29" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="1" t="s">
         <v>75</v>
       </c>
       <c r="G29">
@@ -2050,13 +2050,13 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O29" s="5" t="s">
+      <c r="O29" s="1" t="s">
         <v>65</v>
       </c>
       <c r="P29">
         <v>4</v>
       </c>
-      <c r="Q29" s="5">
+      <c r="Q29" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2065,26 +2065,26 @@
       <c r="B30" t="s">
         <v>76</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E30" s="26"/>
-      <c r="F30" s="5" t="s">
+      <c r="E30" s="22"/>
+      <c r="F30" s="1" t="s">
         <v>77</v>
       </c>
       <c r="G30">
         <v>20</v>
       </c>
       <c r="H30">
-        <f>E11</f>
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <f>E13</f>
         <v>1</v>
       </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
-      <c r="J30">
-        <v>0</v>
-      </c>
       <c r="K30">
         <v>0</v>
       </c>
@@ -2098,13 +2098,13 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="O30" s="5" t="s">
+      <c r="O30" s="1" t="s">
         <v>65</v>
       </c>
       <c r="P30">
         <v>5</v>
       </c>
-      <c r="Q30" s="5">
+      <c r="Q30" s="1">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
@@ -2113,13 +2113,13 @@
       <c r="B31" t="s">
         <v>78</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E31" s="26" t="s">
+      <c r="E31" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="F31" s="5"/>
+      <c r="F31" s="1"/>
       <c r="G31">
         <v>3</v>
       </c>
@@ -2146,13 +2146,13 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O31" s="5" t="s">
+      <c r="O31" s="1" t="s">
         <v>65</v>
       </c>
       <c r="P31">
         <v>2</v>
       </c>
-      <c r="Q31" s="5">
+      <c r="Q31" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2167,10 +2167,10 @@
       <c r="D32">
         <v>16</v>
       </c>
-      <c r="E32" s="26" t="s">
+      <c r="E32" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="F32" s="5"/>
+      <c r="F32" s="1"/>
       <c r="G32">
         <v>5</v>
       </c>
@@ -2196,13 +2196,13 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O32" s="5" t="s">
+      <c r="O32" s="1" t="s">
         <v>59</v>
       </c>
       <c r="P32">
         <v>3</v>
       </c>
-      <c r="Q32" s="5">
+      <c r="Q32" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2214,8 +2214,8 @@
       <c r="C33" t="s">
         <v>80</v>
       </c>
-      <c r="E33" s="26"/>
-      <c r="F33" s="5" t="s">
+      <c r="E33" s="22"/>
+      <c r="F33" s="1" t="s">
         <v>83</v>
       </c>
       <c r="G33">
@@ -2243,13 +2243,13 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O33" s="5" t="s">
+      <c r="O33" s="1" t="s">
         <v>65</v>
       </c>
       <c r="P33">
         <v>3</v>
       </c>
-      <c r="Q33" s="5">
+      <c r="Q33" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2261,8 +2261,8 @@
       <c r="C34" t="s">
         <v>85</v>
       </c>
-      <c r="E34" s="26"/>
-      <c r="F34" s="5" t="s">
+      <c r="E34" s="22"/>
+      <c r="F34" s="1" t="s">
         <v>86</v>
       </c>
       <c r="G34">
@@ -2272,6 +2272,7 @@
         <v>1</v>
       </c>
       <c r="I34">
+        <f>'Hired swords'!B18</f>
         <v>0</v>
       </c>
       <c r="J34">
@@ -2290,13 +2291,13 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="O34" s="5" t="s">
+      <c r="O34" s="1" t="s">
         <v>59</v>
       </c>
       <c r="P34">
         <v>1</v>
       </c>
-      <c r="Q34" s="5">
+      <c r="Q34" s="1">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -2308,8 +2309,8 @@
       <c r="C35" t="s">
         <v>85</v>
       </c>
-      <c r="E35" s="26"/>
-      <c r="F35" s="5" t="s">
+      <c r="E35" s="22"/>
+      <c r="F35" s="1" t="s">
         <v>88</v>
       </c>
       <c r="G35">
@@ -2319,6 +2320,7 @@
         <v>1</v>
       </c>
       <c r="I35">
+        <f>'Hired swords'!B18</f>
         <v>0</v>
       </c>
       <c r="J35">
@@ -2337,27 +2339,27 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="O35" s="5" t="s">
+      <c r="O35" s="1" t="s">
         <v>65</v>
       </c>
       <c r="P35">
         <v>2</v>
       </c>
-      <c r="Q35" s="5">
+      <c r="Q35" s="1">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B36" s="22" t="s">
+      <c r="B36" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="C36" s="22" t="s">
+      <c r="C36" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="D36" s="22"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="22" t="s">
+      <c r="D36" s="18"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="18" t="s">
         <v>91</v>
       </c>
       <c r="G36">
@@ -2385,13 +2387,13 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O36" s="5" t="s">
+      <c r="O36" s="1" t="s">
         <v>59</v>
       </c>
       <c r="P36">
         <v>3</v>
       </c>
-      <c r="Q36" s="5">
+      <c r="Q36" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2403,7 +2405,7 @@
       <c r="C37" t="s">
         <v>93</v>
       </c>
-      <c r="F37" s="26" t="s">
+      <c r="F37" s="22" t="s">
         <v>94</v>
       </c>
       <c r="G37">
@@ -2431,13 +2433,13 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O37" s="5" t="s">
+      <c r="O37" s="1" t="s">
         <v>65</v>
       </c>
       <c r="P37">
         <v>2</v>
       </c>
-      <c r="Q37" s="5">
+      <c r="Q37" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2446,14 +2448,14 @@
       <c r="B38" t="s">
         <v>95</v>
       </c>
-      <c r="C38" s="22" t="s">
+      <c r="C38" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="D38" s="22"/>
-      <c r="E38" s="27" t="s">
+      <c r="D38" s="18"/>
+      <c r="E38" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="F38" s="22" t="s">
+      <c r="F38" s="18" t="s">
         <v>98</v>
       </c>
       <c r="G38">
@@ -2463,7 +2465,7 @@
         <v>1</v>
       </c>
       <c r="I38">
-        <f>I22</f>
+        <f>'Hired swords'!B18</f>
         <v>0</v>
       </c>
       <c r="J38">
@@ -2483,27 +2485,27 @@
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="O38" s="5" t="s">
+      <c r="O38" s="1" t="s">
         <v>65</v>
       </c>
       <c r="P38">
         <v>5</v>
       </c>
-      <c r="Q38" s="5">
+      <c r="Q38" s="1">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C39" s="22" t="s">
+      <c r="C39" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="D39" s="22"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="22" t="s">
+      <c r="D39" s="18"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="18" t="s">
         <v>100</v>
       </c>
       <c r="G39">
@@ -2532,31 +2534,31 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="O39" s="5" t="s">
+      <c r="O39" s="1" t="s">
         <v>33</v>
       </c>
       <c r="P39">
         <v>2</v>
       </c>
-      <c r="Q39" s="5">
+      <c r="Q39" s="1">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C40" s="22" t="s">
+      <c r="C40" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D40" s="22">
+      <c r="D40" s="18">
         <v>8</v>
       </c>
-      <c r="E40" s="26" t="s">
+      <c r="E40" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="F40" s="22" t="s">
+      <c r="F40" s="18" t="s">
         <v>102</v>
       </c>
       <c r="G40">
@@ -2585,77 +2587,77 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="O40" s="5" t="s">
+      <c r="O40" s="1" t="s">
         <v>36</v>
       </c>
       <c r="P40">
         <v>3</v>
       </c>
-      <c r="Q40" s="5">
+      <c r="Q40" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="E41" s="26"/>
+      <c r="E41" s="22"/>
     </row>
     <row r="42" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E42" s="26"/>
-      <c r="H42" s="28">
+      <c r="E42" s="22"/>
+      <c r="H42" s="24">
         <f>H22*$G22+H23*$G23+H24*$G24+H25*$G25+H26*$G26+H27*$G27+H28*$G28+H29*$G29+H30*$G30+H31*$G31+H32*$G32+H33*$G33+H34*$G34+H35*$G35+H36*$G36+H37*$G37+H38*$G38+H39*$G39+G40*H40</f>
-        <v>90</v>
-      </c>
-      <c r="I42" s="28">
+        <v>75</v>
+      </c>
+      <c r="I42" s="24">
         <f>I22*$G22+I23*$G23+I24*$G24+I25*$G25+I26*$G26+I27*$G27+I28*$G28+I29*$G29+I30*$G30+I31*$G31+I32*$G32+I33*$G33+I34*$G34+I35*$G35+I36*$G36+I37*$G37+I38*$G38+I39*$G39+G40*I40</f>
         <v>0</v>
       </c>
-      <c r="J42" s="28">
+      <c r="J42" s="24">
         <f>J22*$G22+J23*$G23+J24*$G24+J25*$G25+J26*$G26+J27*$G27+J28*$G28+J29*$G29+J30*$G30+J31*$G31+J32*$G32+J33*$G33+J34*$G34+J35*$G35+J36*$G36+J37*$G37+J38*$G38+J39*$G39+G40*J40</f>
-        <v>95</v>
-      </c>
-      <c r="K42" s="28">
+        <v>115</v>
+      </c>
+      <c r="K42" s="24">
         <f>K22*$G22+K23*$G23+K24*$G24+K25*$G25+K26*$G26+K27*$G27+K28*$G28+K29*$G29+K30*$G30+K31*$G31+K32*$G32+K33*$G33+K34*$G34+K35*$G35+K36*$G36+K37*$G37+K38*$G38+K39*$G39+G40*K40</f>
         <v>0</v>
       </c>
-      <c r="L42" s="28">
+      <c r="L42" s="24">
         <f>L22*$G22+L23*$G23+L24*$G24+L25*$G25+L26*$G26+L27*$G27+L28*$G28+L29*$G29+L30*$G30+L31*$G31+L32*$G32+L33*$G33+L34*$G34+L35*$G35+L36*$G36+L37*$G37+L38*$G38+L39*$G39+G40*L40</f>
         <v>17</v>
       </c>
-      <c r="M42" s="28">
+      <c r="M42" s="24">
         <f>M22*$G22+M23*$G23+M24*$G24+M25*$G25+M26*$G26+M27*$G27+M28*$G28+M29*$G29+M30*$G30+M31*$G31+M32*$G32+M33*$G33+M34*$G34+M35*$G35+M36*$G36+M37*$G37+M38*$G38+M39*$G39+G40*M40</f>
         <v>0</v>
       </c>
-      <c r="N42" s="11">
+      <c r="N42" s="7">
         <f>SUM(N22:N40)</f>
-        <v>202</v>
-      </c>
-      <c r="O42" s="24"/>
+        <v>207</v>
+      </c>
+      <c r="O42" s="20"/>
       <c r="P42" t="s">
         <v>103</v>
       </c>
-      <c r="Q42" s="11">
+      <c r="Q42" s="7">
         <f>SUM(Tabelle2[Warband Equip Rating])</f>
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B43" s="22"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="24"/>
-      <c r="O43" s="5"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="20"/>
+      <c r="O43" s="1"/>
       <c r="P43" t="s">
         <v>104</v>
       </c>
       <c r="Q43">
         <f>SUM(Q22:Q40)-Q44</f>
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="O44" s="5"/>
+      <c r="O44" s="1"/>
       <c r="P44" t="s">
         <v>105</v>
       </c>
@@ -2685,7 +2687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:U11"/>
   <sheetViews>
-    <sheetView zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
@@ -2699,61 +2701,61 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="O2" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="P2" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="Q2" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="R2" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="S2" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="T2" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="U2" s="4" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2836,79 +2838,79 @@
       </c>
     </row>
     <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.2">
-      <c r="C4" s="29">
+      <c r="C4" s="25">
         <f t="shared" ref="C4:U4" si="1">IF(B10&lt;C3,$A10,IF(B9&lt;C3,$A9,IF(B8&lt;C3,$A8,IF(B7&lt;C3,$A7,IF(B6&lt;C3,$A6,1)))))</f>
         <v>5</v>
       </c>
-      <c r="D4" s="29">
+      <c r="D4" s="25">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="E4" s="29">
+      <c r="E4" s="25">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="F4" s="25">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="F4" s="29">
+      <c r="G4" s="25">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="G4" s="29">
+      <c r="H4" s="25">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="H4" s="29">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="I4" s="29">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="J4" s="29">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="K4" s="29">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="L4" s="29">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="M4" s="29">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="N4" s="29">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="O4" s="29">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="P4" s="29">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="Q4" s="29">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="R4" s="29">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="S4" s="29">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="T4" s="29">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="U4" s="29">
+      <c r="I4" s="25">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J4" s="25">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="K4" s="25">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="L4" s="25">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="M4" s="25">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="N4" s="25">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="O4" s="25">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="P4" s="25">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="Q4" s="25">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="R4" s="25">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="S4" s="25">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="T4" s="25">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="U4" s="25">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -2916,83 +2918,83 @@
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B5">
         <f>'cost calculation'!J6</f>
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C5">
         <f t="shared" ref="C5:U5" si="2">B5+3*C4</f>
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="D5">
         <f t="shared" si="2"/>
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="E5">
         <f t="shared" si="2"/>
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="F5">
         <f t="shared" si="2"/>
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="G5">
         <f t="shared" si="2"/>
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="H5">
         <f t="shared" si="2"/>
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I5">
         <f t="shared" si="2"/>
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J5">
         <f t="shared" si="2"/>
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K5">
         <f t="shared" si="2"/>
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L5">
         <f t="shared" si="2"/>
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M5">
         <f t="shared" si="2"/>
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N5">
         <f t="shared" si="2"/>
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O5">
         <f t="shared" si="2"/>
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="P5">
         <f t="shared" si="2"/>
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Q5">
         <f t="shared" si="2"/>
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="R5">
         <f t="shared" si="2"/>
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="S5">
         <f t="shared" si="2"/>
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="T5">
         <f t="shared" si="2"/>
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="U5">
         <f t="shared" si="2"/>
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
@@ -3001,83 +3003,83 @@
       </c>
       <c r="B6">
         <f t="shared" ref="B6:U6" si="3">B$5+B$5*50%</f>
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="C6">
         <f t="shared" si="3"/>
-        <v>124.5</v>
+        <v>109.5</v>
       </c>
       <c r="D6">
         <f t="shared" si="3"/>
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="E6">
         <f t="shared" si="3"/>
-        <v>165</v>
+        <v>154.5</v>
       </c>
       <c r="F6">
         <f t="shared" si="3"/>
-        <v>183</v>
+        <v>172.5</v>
       </c>
       <c r="G6">
         <f t="shared" si="3"/>
-        <v>201</v>
+        <v>190.5</v>
       </c>
       <c r="H6">
         <f t="shared" si="3"/>
-        <v>214.5</v>
+        <v>208.5</v>
       </c>
       <c r="I6">
         <f t="shared" si="3"/>
-        <v>228</v>
+        <v>226.5</v>
       </c>
       <c r="J6">
         <f t="shared" si="3"/>
-        <v>241.5</v>
+        <v>240</v>
       </c>
       <c r="K6">
         <f t="shared" si="3"/>
-        <v>255</v>
+        <v>253.5</v>
       </c>
       <c r="L6">
         <f t="shared" si="3"/>
-        <v>268.5</v>
+        <v>267</v>
       </c>
       <c r="M6">
         <f t="shared" si="3"/>
-        <v>282</v>
+        <v>280.5</v>
       </c>
       <c r="N6">
         <f t="shared" si="3"/>
-        <v>295.5</v>
+        <v>294</v>
       </c>
       <c r="O6">
         <f t="shared" si="3"/>
-        <v>309</v>
+        <v>307.5</v>
       </c>
       <c r="P6">
         <f t="shared" si="3"/>
-        <v>322.5</v>
+        <v>321</v>
       </c>
       <c r="Q6">
         <f t="shared" si="3"/>
-        <v>336</v>
+        <v>334.5</v>
       </c>
       <c r="R6">
         <f t="shared" si="3"/>
-        <v>349.5</v>
+        <v>348</v>
       </c>
       <c r="S6">
         <f t="shared" si="3"/>
-        <v>363</v>
+        <v>361.5</v>
       </c>
       <c r="T6">
         <f t="shared" si="3"/>
-        <v>376.5</v>
+        <v>375</v>
       </c>
       <c r="U6">
         <f t="shared" si="3"/>
-        <v>390</v>
+        <v>388.5</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
@@ -3086,83 +3088,83 @@
       </c>
       <c r="B7">
         <f t="shared" ref="B7:U7" si="4">B$5+B$5*75%</f>
-        <v>119</v>
+        <v>101.5</v>
       </c>
       <c r="C7">
         <f t="shared" si="4"/>
-        <v>145.25</v>
+        <v>127.75</v>
       </c>
       <c r="D7">
         <f t="shared" si="4"/>
-        <v>171.5</v>
+        <v>154</v>
       </c>
       <c r="E7">
         <f t="shared" si="4"/>
-        <v>192.5</v>
+        <v>180.25</v>
       </c>
       <c r="F7">
         <f t="shared" si="4"/>
-        <v>213.5</v>
+        <v>201.25</v>
       </c>
       <c r="G7">
         <f t="shared" si="4"/>
-        <v>234.5</v>
+        <v>222.25</v>
       </c>
       <c r="H7">
         <f t="shared" si="4"/>
-        <v>250.25</v>
+        <v>243.25</v>
       </c>
       <c r="I7">
         <f t="shared" si="4"/>
-        <v>266</v>
+        <v>264.25</v>
       </c>
       <c r="J7">
         <f t="shared" si="4"/>
-        <v>281.75</v>
+        <v>280</v>
       </c>
       <c r="K7">
         <f t="shared" si="4"/>
-        <v>297.5</v>
+        <v>295.75</v>
       </c>
       <c r="L7">
         <f t="shared" si="4"/>
-        <v>313.25</v>
+        <v>311.5</v>
       </c>
       <c r="M7">
         <f t="shared" si="4"/>
-        <v>329</v>
+        <v>327.25</v>
       </c>
       <c r="N7">
         <f t="shared" si="4"/>
-        <v>344.75</v>
+        <v>343</v>
       </c>
       <c r="O7">
         <f t="shared" si="4"/>
-        <v>360.5</v>
+        <v>358.75</v>
       </c>
       <c r="P7">
         <f t="shared" si="4"/>
-        <v>376.25</v>
+        <v>374.5</v>
       </c>
       <c r="Q7">
         <f t="shared" si="4"/>
-        <v>392</v>
+        <v>390.25</v>
       </c>
       <c r="R7">
         <f t="shared" si="4"/>
-        <v>407.75</v>
+        <v>406</v>
       </c>
       <c r="S7">
         <f t="shared" si="4"/>
-        <v>423.5</v>
+        <v>421.75</v>
       </c>
       <c r="T7">
         <f t="shared" si="4"/>
-        <v>439.25</v>
+        <v>437.5</v>
       </c>
       <c r="U7">
         <f t="shared" si="4"/>
-        <v>455</v>
+        <v>453.25</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
@@ -3171,83 +3173,83 @@
       </c>
       <c r="B8">
         <f t="shared" ref="B8:U8" si="5">B$5+B$5*100%</f>
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="C8">
         <f t="shared" si="5"/>
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="D8">
         <f t="shared" si="5"/>
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="E8">
         <f t="shared" si="5"/>
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="F8">
         <f t="shared" si="5"/>
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="G8">
         <f t="shared" si="5"/>
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="H8">
         <f t="shared" si="5"/>
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="I8">
         <f t="shared" si="5"/>
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J8">
         <f t="shared" si="5"/>
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="K8">
         <f t="shared" si="5"/>
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="L8">
         <f t="shared" si="5"/>
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="M8">
         <f t="shared" si="5"/>
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="N8">
         <f t="shared" si="5"/>
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="O8">
         <f t="shared" si="5"/>
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="P8">
         <f t="shared" si="5"/>
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="Q8">
         <f t="shared" si="5"/>
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="R8">
         <f t="shared" si="5"/>
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="S8">
         <f t="shared" si="5"/>
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="T8">
         <f t="shared" si="5"/>
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="U8">
         <f t="shared" si="5"/>
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
@@ -3256,83 +3258,83 @@
       </c>
       <c r="B9">
         <f t="shared" ref="B9:U9" si="6">B$5+B$5*150%</f>
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="C9">
         <f t="shared" si="6"/>
-        <v>207.5</v>
+        <v>182.5</v>
       </c>
       <c r="D9">
         <f t="shared" si="6"/>
-        <v>245</v>
+        <v>220</v>
       </c>
       <c r="E9">
         <f t="shared" si="6"/>
-        <v>275</v>
+        <v>257.5</v>
       </c>
       <c r="F9">
         <f t="shared" si="6"/>
-        <v>305</v>
+        <v>287.5</v>
       </c>
       <c r="G9">
         <f t="shared" si="6"/>
-        <v>335</v>
+        <v>317.5</v>
       </c>
       <c r="H9">
         <f t="shared" si="6"/>
-        <v>357.5</v>
+        <v>347.5</v>
       </c>
       <c r="I9">
         <f t="shared" si="6"/>
-        <v>380</v>
+        <v>377.5</v>
       </c>
       <c r="J9">
         <f t="shared" si="6"/>
-        <v>402.5</v>
+        <v>400</v>
       </c>
       <c r="K9">
         <f t="shared" si="6"/>
-        <v>425</v>
+        <v>422.5</v>
       </c>
       <c r="L9">
         <f t="shared" si="6"/>
-        <v>447.5</v>
+        <v>445</v>
       </c>
       <c r="M9">
         <f t="shared" si="6"/>
-        <v>470</v>
+        <v>467.5</v>
       </c>
       <c r="N9">
         <f t="shared" si="6"/>
-        <v>492.5</v>
+        <v>490</v>
       </c>
       <c r="O9">
         <f t="shared" si="6"/>
-        <v>515</v>
+        <v>512.5</v>
       </c>
       <c r="P9">
         <f t="shared" si="6"/>
-        <v>537.5</v>
+        <v>535</v>
       </c>
       <c r="Q9">
         <f t="shared" si="6"/>
-        <v>560</v>
+        <v>557.5</v>
       </c>
       <c r="R9">
         <f t="shared" si="6"/>
-        <v>582.5</v>
+        <v>580</v>
       </c>
       <c r="S9">
         <f t="shared" si="6"/>
-        <v>605</v>
+        <v>602.5</v>
       </c>
       <c r="T9">
         <f t="shared" si="6"/>
-        <v>627.5</v>
+        <v>625</v>
       </c>
       <c r="U9">
         <f t="shared" si="6"/>
-        <v>650</v>
+        <v>647.5</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
@@ -3341,159 +3343,159 @@
       </c>
       <c r="B10">
         <f t="shared" ref="B10:U10" si="7">B$5+B$5*300%</f>
-        <v>272</v>
+        <v>232</v>
       </c>
       <c r="C10">
         <f t="shared" si="7"/>
-        <v>332</v>
+        <v>292</v>
       </c>
       <c r="D10">
         <f t="shared" si="7"/>
-        <v>392</v>
+        <v>352</v>
       </c>
       <c r="E10">
         <f t="shared" si="7"/>
-        <v>440</v>
+        <v>412</v>
       </c>
       <c r="F10">
         <f t="shared" si="7"/>
-        <v>488</v>
+        <v>460</v>
       </c>
       <c r="G10">
         <f t="shared" si="7"/>
-        <v>536</v>
+        <v>508</v>
       </c>
       <c r="H10">
         <f t="shared" si="7"/>
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="I10">
         <f t="shared" si="7"/>
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="J10">
         <f t="shared" si="7"/>
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="K10">
         <f t="shared" si="7"/>
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="L10">
         <f t="shared" si="7"/>
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="M10">
         <f t="shared" si="7"/>
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="N10">
         <f t="shared" si="7"/>
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="O10">
         <f t="shared" si="7"/>
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="P10">
         <f t="shared" si="7"/>
-        <v>860</v>
+        <v>856</v>
       </c>
       <c r="Q10">
         <f t="shared" si="7"/>
-        <v>896</v>
+        <v>892</v>
       </c>
       <c r="R10">
         <f t="shared" si="7"/>
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="S10">
         <f t="shared" si="7"/>
-        <v>968</v>
+        <v>964</v>
       </c>
       <c r="T10">
         <f t="shared" si="7"/>
-        <v>1004</v>
+        <v>1000</v>
       </c>
       <c r="U10">
         <f t="shared" si="7"/>
-        <v>1040</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15" x14ac:dyDescent="0.2">
-      <c r="C11" s="29">
+      <c r="C11" s="25">
         <f>C4*'cost calculation'!$E18</f>
         <v>15</v>
       </c>
-      <c r="D11" s="29">
+      <c r="D11" s="25">
         <f>D4*'cost calculation'!$E18</f>
         <v>15</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="25">
         <f>E4*'cost calculation'!$E18</f>
-        <v>12</v>
-      </c>
-      <c r="F11" s="29">
+        <v>15</v>
+      </c>
+      <c r="F11" s="25">
         <f>F4*'cost calculation'!$E18</f>
         <v>12</v>
       </c>
-      <c r="G11" s="29">
+      <c r="G11" s="25">
         <f>G4*'cost calculation'!$E18</f>
         <v>12</v>
       </c>
-      <c r="H11" s="29">
+      <c r="H11" s="25">
         <f>H4*'cost calculation'!$E18</f>
-        <v>9</v>
-      </c>
-      <c r="I11" s="29">
+        <v>12</v>
+      </c>
+      <c r="I11" s="25">
         <f>I4*'cost calculation'!$E18</f>
-        <v>9</v>
-      </c>
-      <c r="J11" s="29">
+        <v>12</v>
+      </c>
+      <c r="J11" s="25">
         <f>J4*'cost calculation'!$E18</f>
         <v>9</v>
       </c>
-      <c r="K11" s="29">
+      <c r="K11" s="25">
         <f>K4*'cost calculation'!$E18</f>
         <v>9</v>
       </c>
-      <c r="L11" s="29">
+      <c r="L11" s="25">
         <f>L4*'cost calculation'!$E18</f>
         <v>9</v>
       </c>
-      <c r="M11" s="29">
+      <c r="M11" s="25">
         <f>M4*'cost calculation'!$E18</f>
         <v>9</v>
       </c>
-      <c r="N11" s="29">
+      <c r="N11" s="25">
         <f>N4*'cost calculation'!$E18</f>
         <v>9</v>
       </c>
-      <c r="O11" s="29">
+      <c r="O11" s="25">
         <f>O4*'cost calculation'!$E18</f>
         <v>9</v>
       </c>
-      <c r="P11" s="29">
+      <c r="P11" s="25">
         <f>P4*'cost calculation'!$E18</f>
         <v>9</v>
       </c>
-      <c r="Q11" s="29">
+      <c r="Q11" s="25">
         <f>Q4*'cost calculation'!$E18</f>
         <v>9</v>
       </c>
-      <c r="R11" s="29">
+      <c r="R11" s="25">
         <f>R4*'cost calculation'!$E18</f>
         <v>9</v>
       </c>
-      <c r="S11" s="29">
+      <c r="S11" s="25">
         <f>S4*'cost calculation'!$E18</f>
         <v>9</v>
       </c>
-      <c r="T11" s="29">
+      <c r="T11" s="25">
         <f>T4*'cost calculation'!$E18</f>
         <v>9</v>
       </c>
-      <c r="U11" s="29">
+      <c r="U11" s="25">
         <f>U4*'cost calculation'!$E18</f>
         <v>9</v>
       </c>
@@ -3508,8 +3510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:O19"/>
   <sheetViews>
-    <sheetView zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3533,46 +3535,46 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="L2" s="30" t="s">
+      <c r="L2" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="M2" s="30" t="s">
+      <c r="M2" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="N2" s="31" t="s">
+      <c r="N2" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="1" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3604,18 +3606,18 @@
         <f t="shared" ref="I3:I18" si="2">F3*B3</f>
         <v>0</v>
       </c>
-      <c r="J3" s="32">
+      <c r="J3" s="28">
         <f t="shared" ref="J3:J18" si="3">F3/D3</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="K3" s="32">
+      <c r="K3" s="28">
         <f t="shared" ref="K3:K18" si="4">F3/E3</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="L3" s="33" t="s">
+      <c r="L3" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="M3" s="33"/>
+      <c r="M3" s="29"/>
       <c r="N3">
         <v>3</v>
       </c>
@@ -3652,18 +3654,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J4" s="32">
+      <c r="J4" s="28">
         <f t="shared" si="3"/>
         <v>0.73333333333333328</v>
       </c>
-      <c r="K4" s="32">
+      <c r="K4" s="28">
         <f t="shared" si="4"/>
         <v>1.4666666666666666</v>
       </c>
-      <c r="L4" s="33" t="s">
+      <c r="L4" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="M4" s="33"/>
+      <c r="M4" s="29"/>
       <c r="N4">
         <v>3</v>
       </c>
@@ -3700,18 +3702,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J5" s="32">
+      <c r="J5" s="28">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K5" s="32">
+      <c r="K5" s="28">
         <f t="shared" si="4"/>
         <v>1.3333333333333333</v>
       </c>
-      <c r="L5" s="33" t="s">
+      <c r="L5" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="M5" s="33"/>
+      <c r="M5" s="29"/>
       <c r="N5">
         <v>3</v>
       </c>
@@ -3748,18 +3750,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J6" s="32">
+      <c r="J6" s="28">
         <f t="shared" si="3"/>
         <v>0.51428571428571423</v>
       </c>
-      <c r="K6" s="32">
+      <c r="K6" s="28">
         <f t="shared" si="4"/>
         <v>1.2</v>
       </c>
-      <c r="L6" s="33" t="s">
+      <c r="L6" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="M6" s="33"/>
+      <c r="M6" s="29"/>
       <c r="N6">
         <v>3</v>
       </c>
@@ -3796,18 +3798,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J7" s="32">
+      <c r="J7" s="28">
         <f t="shared" si="3"/>
         <v>0.44444444444444442</v>
       </c>
-      <c r="K7" s="32">
+      <c r="K7" s="28">
         <f t="shared" si="4"/>
         <v>1.1428571428571428</v>
       </c>
-      <c r="L7" s="33" t="s">
+      <c r="L7" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="M7" s="33"/>
+      <c r="M7" s="29"/>
       <c r="N7">
         <v>5</v>
       </c>
@@ -3844,18 +3846,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J8" s="32">
+      <c r="J8" s="28">
         <f t="shared" si="3"/>
         <v>0.53333333333333333</v>
       </c>
-      <c r="K8" s="32">
+      <c r="K8" s="28">
         <f t="shared" si="4"/>
         <v>1.0666666666666667</v>
       </c>
-      <c r="L8" s="33" t="s">
+      <c r="L8" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="M8" s="33"/>
+      <c r="M8" s="29"/>
       <c r="N8">
         <v>2</v>
       </c>
@@ -3892,18 +3894,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J9" s="32">
+      <c r="J9" s="28">
         <f t="shared" si="3"/>
         <v>0.625</v>
       </c>
-      <c r="K9" s="32">
+      <c r="K9" s="28">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="L9" s="33" t="s">
+      <c r="L9" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="M9" s="33"/>
+      <c r="M9" s="29"/>
       <c r="N9">
         <v>4</v>
       </c>
@@ -3940,18 +3942,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J10" s="32">
+      <c r="J10" s="28">
         <f t="shared" si="3"/>
         <v>0.41666666666666669</v>
       </c>
-      <c r="K10" s="32">
+      <c r="K10" s="28">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="L10" s="33" t="s">
+      <c r="L10" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="M10" s="33"/>
+      <c r="M10" s="29"/>
       <c r="N10">
         <v>3</v>
       </c>
@@ -3988,18 +3990,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J11" s="32">
+      <c r="J11" s="28">
         <f t="shared" si="3"/>
         <v>0.35714285714285715</v>
       </c>
-      <c r="K11" s="32">
+      <c r="K11" s="28">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="L11" s="33" t="s">
+      <c r="L11" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="M11" s="33"/>
+      <c r="M11" s="29"/>
       <c r="N11">
         <v>3</v>
       </c>
@@ -4036,18 +4038,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J12" s="32">
+      <c r="J12" s="28">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K12" s="32">
+      <c r="K12" s="28">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="L12" s="33" t="s">
+      <c r="L12" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="M12" s="33"/>
+      <c r="M12" s="29"/>
       <c r="N12">
         <v>3</v>
       </c>
@@ -4084,18 +4086,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J13" s="32">
+      <c r="J13" s="28">
         <f t="shared" si="3"/>
         <v>0.23076923076923078</v>
       </c>
-      <c r="K13" s="32">
+      <c r="K13" s="28">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="L13" s="33" t="s">
+      <c r="L13" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="M13" s="33"/>
+      <c r="M13" s="29"/>
       <c r="N13">
         <v>2</v>
       </c>
@@ -4132,18 +4134,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J14" s="32">
+      <c r="J14" s="28">
         <f t="shared" si="3"/>
         <v>0.46666666666666667</v>
       </c>
-      <c r="K14" s="32">
+      <c r="K14" s="28">
         <f t="shared" si="4"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="L14" s="33" t="s">
+      <c r="L14" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="M14" s="33"/>
+      <c r="M14" s="29"/>
       <c r="N14">
         <v>2</v>
       </c>
@@ -4180,18 +4182,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J15" s="32">
+      <c r="J15" s="28">
         <f t="shared" si="3"/>
         <v>0.3125</v>
       </c>
-      <c r="K15" s="32">
+      <c r="K15" s="28">
         <f t="shared" si="4"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="L15" s="33" t="s">
+      <c r="L15" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="M15" s="33"/>
+      <c r="M15" s="29"/>
       <c r="N15">
         <v>0</v>
       </c>
@@ -4228,18 +4230,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J16" s="32">
+      <c r="J16" s="28">
         <f t="shared" si="3"/>
         <v>0.3</v>
       </c>
-      <c r="K16" s="32">
+      <c r="K16" s="28">
         <f t="shared" si="4"/>
         <v>0.75</v>
       </c>
-      <c r="L16" s="33" t="s">
+      <c r="L16" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="M16" s="33"/>
+      <c r="M16" s="29"/>
       <c r="N16">
         <v>3</v>
       </c>
@@ -4276,18 +4278,18 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J17" s="32">
+      <c r="J17" s="28">
         <f t="shared" si="3"/>
         <v>0.35714285714285715</v>
       </c>
-      <c r="K17" s="32">
+      <c r="K17" s="28">
         <f t="shared" si="4"/>
         <v>0.7142857142857143</v>
       </c>
-      <c r="L17" s="33" t="s">
+      <c r="L17" s="29" t="s">
         <v>166</v>
       </c>
-      <c r="M17" s="33"/>
+      <c r="M17" s="29"/>
       <c r="N17">
         <v>4</v>
       </c>
@@ -4298,7 +4300,7 @@
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" t="s">
         <v>167</v>
@@ -4314,56 +4316,56 @@
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="H18">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I18">
         <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="J18" s="32">
+        <v>0</v>
+      </c>
+      <c r="J18" s="28">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="K18" s="32">
+      <c r="K18" s="28">
         <f t="shared" si="4"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="L18" s="33" t="s">
+      <c r="L18" s="29" t="s">
         <v>168</v>
       </c>
-      <c r="M18" s="33"/>
+      <c r="M18" s="29"/>
       <c r="N18">
         <v>2</v>
       </c>
       <c r="O18">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B19" s="8">
+      <c r="B19" s="4">
         <f>SUM(B3:B18)</f>
-        <v>1</v>
-      </c>
-      <c r="G19" s="8">
+        <v>0</v>
+      </c>
+      <c r="G19" s="4">
         <f>SUM(G3:G18)</f>
-        <v>20</v>
-      </c>
-      <c r="H19" s="8">
+        <v>0</v>
+      </c>
+      <c r="H19" s="4">
         <f>SUM(H3:H18)</f>
-        <v>15</v>
-      </c>
-      <c r="I19" s="8">
+        <v>0</v>
+      </c>
+      <c r="I19" s="4">
         <f>SUM(I3:I18)</f>
-        <v>10</v>
-      </c>
-      <c r="O19" s="8">
+        <v>0</v>
+      </c>
+      <c r="O19" s="4">
         <f>SUM(O3:O18)</f>
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4401,66 +4403,66 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="7" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1" t="s">
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="K3" s="2" t="s">
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="K3" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="L3" s="2"/>
+      <c r="L3" s="38"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B4" s="34"/>
-      <c r="C4" s="18" t="str">
+      <c r="B4" s="30"/>
+      <c r="C4" s="14" t="str">
         <f>'cost calculation'!C11</f>
         <v>Chief</v>
       </c>
-      <c r="D4" s="18" t="str">
+      <c r="D4" s="14" t="str">
         <f>'cost calculation'!C12</f>
         <v>Braves (¾)</v>
       </c>
-      <c r="E4" s="18" t="str">
+      <c r="E4" s="14" t="str">
         <f>'cost calculation'!C13</f>
         <v>Shaman</v>
       </c>
-      <c r="F4" s="18" t="str">
+      <c r="F4" s="14" t="str">
         <f>'cost calculation'!C14</f>
         <v>forest goblins</v>
       </c>
-      <c r="G4" s="18" t="str">
+      <c r="G4" s="14" t="str">
         <f>'cost calculation'!C15</f>
         <v>Shootaz (5)</v>
       </c>
-      <c r="H4" s="18" t="str">
+      <c r="H4" s="14" t="str">
         <f>'cost calculation'!C16</f>
         <v>red toof goblinz (5)</v>
       </c>
-      <c r="I4" s="18" t="str">
+      <c r="I4" s="14" t="str">
         <f>'cost calculation'!C17</f>
         <v>giantic spider</v>
       </c>
-      <c r="K4" s="35" t="s">
+      <c r="K4" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="L4" s="36" t="s">
+      <c r="L4" s="32" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="33" t="s">
         <v>171</v>
       </c>
       <c r="C5">
@@ -4475,7 +4477,7 @@
       <c r="F5">
         <v>4</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G5" s="20">
         <v>4</v>
       </c>
       <c r="H5">
@@ -4484,15 +4486,15 @@
       <c r="I5">
         <v>6</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="1">
         <v>4</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="33" t="s">
         <v>172</v>
       </c>
       <c r="C6">
@@ -4516,15 +4518,15 @@
       <c r="I6">
         <v>3</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="1">
         <v>2</v>
       </c>
-      <c r="L6" s="38">
+      <c r="L6" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="33" t="s">
         <v>173</v>
       </c>
       <c r="C7">
@@ -4551,12 +4553,12 @@
       <c r="K7">
         <v>2</v>
       </c>
-      <c r="L7" s="38">
+      <c r="L7" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="33" t="s">
         <v>33</v>
       </c>
       <c r="C8">
@@ -4583,12 +4585,12 @@
       <c r="K8">
         <v>6</v>
       </c>
-      <c r="L8" s="38">
+      <c r="L8" s="34">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="33" t="s">
         <v>174</v>
       </c>
       <c r="C9">
@@ -4612,15 +4614,15 @@
       <c r="I9">
         <v>5</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="1">
         <v>4</v>
       </c>
-      <c r="L9" s="38">
+      <c r="L9" s="34">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="33" t="s">
         <v>175</v>
       </c>
       <c r="C10">
@@ -4644,15 +4646,15 @@
       <c r="I10">
         <v>3</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10" s="1">
         <v>6</v>
       </c>
-      <c r="L10" s="38">
+      <c r="L10" s="34">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="33" t="s">
         <v>176</v>
       </c>
       <c r="C11">
@@ -4679,12 +4681,12 @@
       <c r="K11">
         <v>2</v>
       </c>
-      <c r="L11" s="38">
+      <c r="L11" s="34">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="33" t="s">
         <v>177</v>
       </c>
       <c r="C12">
@@ -4711,12 +4713,12 @@
       <c r="K12">
         <v>6</v>
       </c>
-      <c r="L12" s="38">
+      <c r="L12" s="34">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="33" t="s">
         <v>178</v>
       </c>
       <c r="C13">
@@ -4743,441 +4745,441 @@
       <c r="K13">
         <v>2</v>
       </c>
-      <c r="L13" s="38">
+      <c r="L13" s="34">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B14" s="37"/>
-      <c r="L14" s="38"/>
+      <c r="B14" s="33"/>
+      <c r="L14" s="34"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>179</v>
       </c>
-      <c r="C15" s="39">
+      <c r="C15" s="35">
         <f t="shared" ref="C15:E23" si="0">$K5*C5/C$25</f>
         <v>0.32</v>
       </c>
-      <c r="D15" s="39">
+      <c r="D15" s="35">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="E15" s="39">
+      <c r="E15" s="35">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="F15" s="39">
+      <c r="F15" s="35">
         <f t="shared" ref="F15:I23" si="1">$L5*F5/F$25</f>
         <v>0.8</v>
       </c>
-      <c r="G15" s="39">
+      <c r="G15" s="35">
         <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
-      <c r="H15" s="39">
+      <c r="H15" s="35">
         <f t="shared" si="1"/>
         <v>0.48</v>
       </c>
-      <c r="I15" s="39">
+      <c r="I15" s="35">
         <f t="shared" si="1"/>
         <v>0.09</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="C16" s="39">
+      <c r="C16" s="35">
         <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
-      <c r="D16" s="39">
+      <c r="D16" s="35">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="E16" s="39">
+      <c r="E16" s="35">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="F16" s="39">
+      <c r="F16" s="35">
         <f t="shared" si="1"/>
         <v>0.13333333333333333</v>
       </c>
-      <c r="G16" s="39">
+      <c r="G16" s="35">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="H16" s="39">
+      <c r="H16" s="35">
         <f t="shared" si="1"/>
         <v>0.08</v>
       </c>
-      <c r="I16" s="39">
+      <c r="I16" s="35">
         <f t="shared" si="1"/>
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="C17" s="39">
+      <c r="C17" s="35">
         <f t="shared" si="0"/>
         <v>0.16</v>
       </c>
-      <c r="D17" s="39">
+      <c r="D17" s="35">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="E17" s="39">
+      <c r="E17" s="35">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="F17" s="39">
+      <c r="F17" s="35">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="G17" s="39">
+      <c r="G17" s="35">
         <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
-      <c r="H17" s="39">
+      <c r="H17" s="35">
         <f t="shared" si="1"/>
         <v>0.12</v>
       </c>
-      <c r="I17" s="39">
+      <c r="I17" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="33" t="s">
         <v>182</v>
       </c>
-      <c r="C18" s="39">
+      <c r="C18" s="35">
         <f t="shared" si="0"/>
         <v>0.36</v>
       </c>
-      <c r="D18" s="39">
+      <c r="D18" s="35">
         <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
-      <c r="E18" s="39">
+      <c r="E18" s="35">
         <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
-      <c r="F18" s="39">
+      <c r="F18" s="35">
         <f t="shared" si="1"/>
         <v>1.2</v>
       </c>
-      <c r="G18" s="39">
+      <c r="G18" s="35">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
-      <c r="H18" s="39">
+      <c r="H18" s="35">
         <f t="shared" si="1"/>
         <v>0.72</v>
       </c>
-      <c r="I18" s="39">
+      <c r="I18" s="35">
         <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="C19" s="39">
+      <c r="C19" s="35">
         <f t="shared" si="0"/>
         <v>0.24</v>
       </c>
-      <c r="D19" s="39">
+      <c r="D19" s="35">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-      <c r="E19" s="39">
+      <c r="E19" s="35">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-      <c r="F19" s="39">
+      <c r="F19" s="35">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="G19" s="39">
+      <c r="G19" s="35">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
-      <c r="H19" s="39">
+      <c r="H19" s="35">
         <f t="shared" si="1"/>
         <v>0.24</v>
       </c>
-      <c r="I19" s="39">
+      <c r="I19" s="35">
         <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B20" s="37" t="s">
+      <c r="B20" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="C20" s="39">
+      <c r="C20" s="35">
         <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
-      <c r="D20" s="39">
+      <c r="D20" s="35">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="E20" s="39">
+      <c r="E20" s="35">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="F20" s="39">
+      <c r="F20" s="35">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="G20" s="39">
+      <c r="G20" s="35">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
-      <c r="H20" s="39">
+      <c r="H20" s="35">
         <f t="shared" si="1"/>
         <v>0.24</v>
       </c>
-      <c r="I20" s="39">
+      <c r="I20" s="35">
         <f t="shared" si="1"/>
         <v>0.09</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="C21" s="39">
+      <c r="C21" s="35">
         <f t="shared" si="0"/>
         <v>0.16</v>
       </c>
-      <c r="D21" s="39">
+      <c r="D21" s="35">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="E21" s="39">
+      <c r="E21" s="35">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="F21" s="39">
+      <c r="F21" s="35">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="G21" s="39">
+      <c r="G21" s="35">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
-      <c r="H21" s="39">
+      <c r="H21" s="35">
         <f t="shared" si="1"/>
         <v>0.24</v>
       </c>
-      <c r="I21" s="39">
+      <c r="I21" s="35">
         <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="33" t="s">
         <v>186</v>
       </c>
-      <c r="C22" s="39">
+      <c r="C22" s="35">
         <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
-      <c r="D22" s="39">
+      <c r="D22" s="35">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="E22" s="39">
+      <c r="E22" s="35">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="F22" s="39">
+      <c r="F22" s="35">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="G22" s="39">
+      <c r="G22" s="35">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
-      <c r="H22" s="39">
+      <c r="H22" s="35">
         <f t="shared" si="1"/>
         <v>0.48</v>
       </c>
-      <c r="I22" s="39">
+      <c r="I22" s="35">
         <f t="shared" si="1"/>
         <v>0.06</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B23" s="37" t="s">
+      <c r="B23" s="33" t="s">
         <v>187</v>
       </c>
-      <c r="C23" s="39">
+      <c r="C23" s="35">
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-      <c r="D23" s="39">
+      <c r="D23" s="35">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-      <c r="E23" s="39">
+      <c r="E23" s="35">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-      <c r="F23" s="39">
+      <c r="F23" s="35">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="G23" s="39">
+      <c r="G23" s="35">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
-      <c r="H23" s="39">
+      <c r="H23" s="35">
         <f t="shared" si="1"/>
         <v>0.24</v>
       </c>
-      <c r="I23" s="39">
+      <c r="I23" s="35">
         <f t="shared" si="1"/>
         <v>0.02</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="E24" s="8"/>
+      <c r="E24" s="4"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="1">
         <f>'cost calculation'!D11</f>
         <v>50</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="1">
         <f>'cost calculation'!D12</f>
         <v>20</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="1">
         <f>'cost calculation'!D13</f>
         <v>20</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="1">
         <f>'cost calculation'!D14</f>
         <v>15</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="1">
         <f>'cost calculation'!D15</f>
         <v>20</v>
       </c>
-      <c r="H25" s="5">
+      <c r="H25" s="1">
         <f>'cost calculation'!D16</f>
         <v>25</v>
       </c>
-      <c r="I25" s="5">
+      <c r="I25" s="1">
         <f>'cost calculation'!D17</f>
         <v>200</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C27" s="39">
+      <c r="C27" s="35">
         <f t="shared" ref="C27:I27" si="2">SUM(C15:C23)</f>
         <v>1.8799999999999997</v>
       </c>
-      <c r="D27" s="39">
+      <c r="D27" s="35">
         <f t="shared" si="2"/>
         <v>4.3</v>
       </c>
-      <c r="E27" s="39">
+      <c r="E27" s="35">
         <f t="shared" si="2"/>
         <v>4.3999999999999995</v>
       </c>
-      <c r="F27" s="39">
+      <c r="F27" s="35">
         <f t="shared" si="2"/>
         <v>4.333333333333333</v>
       </c>
-      <c r="G27" s="39">
+      <c r="G27" s="35">
         <f t="shared" si="2"/>
         <v>3.8499999999999992</v>
       </c>
-      <c r="H27" s="39">
+      <c r="H27" s="35">
         <f t="shared" si="2"/>
         <v>2.84</v>
       </c>
-      <c r="I27" s="39">
+      <c r="I27" s="35">
         <f t="shared" si="2"/>
         <v>0.51500000000000001</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C28" s="32">
+      <c r="C28" s="28">
         <f>'cost calculation'!$E11*'Characteristic analysis'!C27</f>
         <v>1.8799999999999997</v>
       </c>
-      <c r="D28" s="32">
+      <c r="D28" s="28">
         <f>'cost calculation'!$E12*'Characteristic analysis'!D27</f>
         <v>0</v>
       </c>
-      <c r="E28" s="32">
+      <c r="E28" s="28">
         <f>'cost calculation'!$E13*'Characteristic analysis'!E27</f>
         <v>4.3999999999999995</v>
       </c>
-      <c r="F28" s="32">
+      <c r="F28" s="28">
         <f>'cost calculation'!$E14*'Characteristic analysis'!F27</f>
         <v>0</v>
       </c>
-      <c r="G28" s="32">
+      <c r="G28" s="28">
         <f>'cost calculation'!$E15*'Characteristic analysis'!G27</f>
         <v>3.8499999999999992</v>
       </c>
-      <c r="H28" s="32">
+      <c r="H28" s="28">
         <f>'cost calculation'!$E16*'Characteristic analysis'!H27</f>
         <v>0</v>
       </c>
-      <c r="I28" s="32">
+      <c r="I28" s="28">
         <f>'cost calculation'!$E17*'Characteristic analysis'!I27</f>
         <v>0</v>
       </c>
-      <c r="J28" s="12">
+      <c r="J28" s="8">
         <f>SUM(C28:I28)</f>
         <v>10.129999999999999</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C29" s="32">
+      <c r="C29" s="28">
         <f>'cost calculation'!$E11*(C5*K5+C6*K6+C7*K7+C8*K8+C9*K9+C10*K10+C11*K11+C12*K12+C13*K13)</f>
         <v>94</v>
       </c>
-      <c r="D29" s="32">
+      <c r="D29" s="28">
         <f>'cost calculation'!$E12*(D5*$L5+D6*$L6+D7*$L7+D8*$L8+D9*$L9+D10*$L10+D11*$L11+D12*$L12+D13*$L13)</f>
         <v>0</v>
       </c>
-      <c r="E29" s="32">
+      <c r="E29" s="28">
         <f>'cost calculation'!$E13*(E5*$L5+E6*$L6+E7*$L7+E8*$L8+E9*$L9+E10*$L10+E11*$L11+E12*$L12+E13*$L13)</f>
         <v>67</v>
       </c>
-      <c r="F29" s="32">
+      <c r="F29" s="28">
         <f>'cost calculation'!$E14*(F5*$L5+F6*$L6+F7*$L7+F8*$L8+F9*$L9+F10*$L10+F11*$L11+F12*$L12+F13*$L13)</f>
         <v>0</v>
       </c>
-      <c r="G29" s="32">
+      <c r="G29" s="28">
         <f>'cost calculation'!$E15*(G5*$L5+G6*$L6+G7*$L7+G8*$L8+G9*$L9+G10*$L10+G11*$L11+G12*$L12+G13*$L13)</f>
         <v>77</v>
       </c>
-      <c r="H29" s="32">
+      <c r="H29" s="28">
         <f>'cost calculation'!$E16*(H5*$L5+H6*$L6+H7*$L7+H8*$L8+H9*$L9+H10*$L10+H11*$L11+H12*$L12+H13*$L13)</f>
         <v>0</v>
       </c>
-      <c r="I29" s="32">
+      <c r="I29" s="28">
         <f>'cost calculation'!$E17*(I5*$L5+I6*$L6+I7*$L7+I8*$L8+I9*$L9+I10*$L10+I11*$L11+I12*$L12+I13*$L13)</f>
         <v>0</v>
       </c>
-      <c r="J29" s="12">
+      <c r="J29" s="8">
         <f>SUM(C29:I29)</f>
         <v>238</v>
       </c>

</xml_diff>